<commit_message>
change to misere 4 times 4 with more hidden layers
</commit_message>
<xml_diff>
--- a/results3times3.xlsx
+++ b/results3times3.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>episode: 362000 win_rate: 0.859</t>
   </si>
@@ -96,6 +96,72 @@
   </si>
   <si>
     <t>episode: 384000 win_rate: 0.82</t>
+  </si>
+  <si>
+    <t>episode: 372000 win_rate: 0.305</t>
+  </si>
+  <si>
+    <t>episode: 373000 win_rate: 0.332</t>
+  </si>
+  <si>
+    <t>episode: 374000 win_rate: 0.322</t>
+  </si>
+  <si>
+    <t>episode: 375000 win_rate: 0.3165</t>
+  </si>
+  <si>
+    <t>episode: 376000 win_rate: 0.319</t>
+  </si>
+  <si>
+    <t>episode: 377000 win_rate: 0.281</t>
+  </si>
+  <si>
+    <t>episode: 378000 win_rate: 0.306</t>
+  </si>
+  <si>
+    <t>episode: 379000 win_rate: 0.307</t>
+  </si>
+  <si>
+    <t>episode: 380000 win_rate: 0.348</t>
+  </si>
+  <si>
+    <t>episode: 381000 win_rate: 0.321</t>
+  </si>
+  <si>
+    <t>episode: 382000 win_rate: 0.319</t>
+  </si>
+  <si>
+    <t>episode: 383000 win_rate: 0.3</t>
+  </si>
+  <si>
+    <t>episode: 384000 win_rate: 0.308</t>
+  </si>
+  <si>
+    <t>episode: 385000 win_rate: 0.3375</t>
+  </si>
+  <si>
+    <t>episode: 386000 win_rate: 0.324</t>
+  </si>
+  <si>
+    <t>episode: 387000 win_rate: 0.3315</t>
+  </si>
+  <si>
+    <t>episode: 388000 win_rate: 0.322</t>
+  </si>
+  <si>
+    <t>episode: 389000 win_rate: 0.331</t>
+  </si>
+  <si>
+    <t>episode: 390000 win_rate: 0.3105</t>
+  </si>
+  <si>
+    <t>episode: 391000 win_rate: 0.322</t>
+  </si>
+  <si>
+    <t>episode: 392000 win_rate: 0.323</t>
+  </si>
+  <si>
+    <t>episode: 393000 win_rate: 0.298</t>
   </si>
 </sst>
 </file>
@@ -416,125 +482,191 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A23"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F3" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F4" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F5" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F6" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F7" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F8" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F9" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F10" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F11" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F12" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F13" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F14" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F15" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F16" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F17" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F18" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F19" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F20" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F21" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F22" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>

</xml_diff>